<commit_message>
[IMP] ENH pabi standard asset
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_standard_asset.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_standard_asset.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
-  <si>
-    <t>สำนักงานพัฒนาวิทยาศาสตร์และเทคโนโลยีแห่งชาติ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>ศูนย์</t>
   </si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>รายงานผลการจัดซื้อครุภัณฑ์มาตรฐาน</t>
-  </si>
-  <si>
-    <t>กระทรวงวิทยาศาสตร์และเทคโนโลยี</t>
   </si>
   <si>
     <t>วงเงินตั้งงบประมาณ</t>
@@ -128,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -251,11 +245,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -286,9 +277,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -325,6 +313,9 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,249 +599,244 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="36.6328125" style="11" customWidth="1"/>
-    <col min="4" max="6" width="20" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" style="9" customWidth="1"/>
-    <col min="8" max="10" width="10.36328125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="11"/>
-    <col min="12" max="13" width="17.26953125" style="11" customWidth="1"/>
-    <col min="14" max="14" width="16.08984375" style="10" customWidth="1"/>
-    <col min="15" max="15" width="13.26953125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="8.81640625" style="10"/>
-    <col min="18" max="18" width="8.81640625" style="11"/>
-    <col min="19" max="19" width="11.90625" style="11" customWidth="1"/>
-    <col min="20" max="20" width="25.81640625" style="11" customWidth="1"/>
-    <col min="21" max="21" width="14.453125" style="11" customWidth="1"/>
-    <col min="22" max="16384" width="8.81640625" style="12"/>
+    <col min="1" max="1" width="16.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="10" customWidth="1"/>
+    <col min="4" max="6" width="20" style="10" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="10.33203125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="10"/>
+    <col min="12" max="13" width="17.33203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" style="9"/>
+    <col min="18" max="18" width="8.83203125" style="10"/>
+    <col min="19" max="19" width="11.83203125" style="10" customWidth="1"/>
+    <col min="20" max="20" width="25.83203125" style="10" customWidth="1"/>
+    <col min="21" max="21" width="14.5" style="10" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+    </row>
+    <row r="2" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:21" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-    </row>
-    <row r="11" spans="1:21" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19" t="s">
+      <c r="O11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="R11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="S11" s="19" t="s">
+      <c r="U11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="U11" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+    </row>
+    <row r="12" spans="1:21" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="15"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A13" s="15"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A14" s="15"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.60972222222222205" bottom="0.37013888888888902" header="0.51180555555555496" footer="0.1"/>

</xml_diff>

<commit_message>
#3438 - edit standard asset report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_standard_asset.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_standard_asset.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="150001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -71,9 +71,6 @@
     <t>ปีที่จัดซื้อ</t>
   </si>
   <si>
-    <t>รายการ</t>
-  </si>
-  <si>
     <t>ยี่ห้อ</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>ราคาที่จัดซื้อ</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
   </si>
 </sst>
 </file>
@@ -124,7 +124,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="187" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -266,7 +266,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -280,7 +280,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -299,7 +299,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -308,7 +308,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -321,8 +321,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -599,34 +627,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="10" customWidth="1"/>
     <col min="4" max="6" width="20" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" customWidth="1"/>
-    <col min="8" max="10" width="10.33203125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="10"/>
-    <col min="12" max="13" width="17.33203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="9" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" style="9" customWidth="1"/>
-    <col min="17" max="17" width="8.83203125" style="9"/>
-    <col min="18" max="18" width="8.83203125" style="10"/>
-    <col min="19" max="19" width="11.83203125" style="10" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" style="10" customWidth="1"/>
-    <col min="21" max="21" width="14.5" style="10" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="11"/>
+    <col min="7" max="7" width="15.28515625" style="8" customWidth="1"/>
+    <col min="8" max="10" width="10.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="10" customWidth="1"/>
+    <col min="12" max="13" width="17.28515625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="9" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="9"/>
+    <col min="18" max="18" width="8.85546875" style="10"/>
+    <col min="19" max="19" width="11.85546875" style="10" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="10" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="10" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -649,7 +677,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -659,7 +687,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -669,9 +697,9 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -679,9 +707,9 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -689,9 +717,9 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -699,9 +727,9 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="7"/>
@@ -709,9 +737,9 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -719,7 +747,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
@@ -732,11 +760,11 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:21" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>3</v>
       </c>
@@ -768,40 +796,40 @@
         <v>12</v>
       </c>
       <c r="K11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="M11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="N11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="Q11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="17" t="s">
+      <c r="R11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="17" t="s">
+      <c r="S11" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="S11" s="17" t="s">
-        <v>19</v>
       </c>
       <c r="T11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="U11" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="11.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>

</xml_diff>